<commit_message>
Added example code for getting a matched value's adjacent cell's values.
</commit_message>
<xml_diff>
--- a/files/excelfile.xlsx
+++ b/files/excelfile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>oneone</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t>threethree</t>
+  </si>
+  <si>
+    <t>4-1</t>
+  </si>
+  <si>
+    <t>4-2</t>
+  </si>
+  <si>
+    <t>4-3</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Firstname Lastname</t>
   </si>
 </sst>
 </file>
@@ -81,8 +99,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,13 +383,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -402,6 +426,28 @@
       </c>
       <c r="C3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>